<commit_message>
add title column and change author to authors
</commit_message>
<xml_diff>
--- a/assets/metadata_template.xlsx
+++ b/assets/metadata_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\kyle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\sample_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C69E3E8-25C8-40EB-994B-84754EE2B1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149D3522-952C-4D1B-B7A1-0870DD324B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata_template" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="282">
   <si>
     <t>Strategy</t>
   </si>
@@ -813,9 +813,6 @@
     <t>sample_name</t>
   </si>
   <si>
-    <t>author</t>
-  </si>
-  <si>
     <t>isolate</t>
   </si>
   <si>
@@ -840,9 +837,6 @@
     <t>test_field_3</t>
   </si>
   <si>
-    <t>fasta_file_name</t>
-  </si>
-  <si>
     <t>ncbi-spuid</t>
   </si>
   <si>
@@ -874,6 +868,18 @@
   </si>
   <si>
     <t>publication_title</t>
+  </si>
+  <si>
+    <t>fasta_path</t>
+  </si>
+  <si>
+    <t>gff_path</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>authors</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1043,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1070,16 +1076,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1094,14 +1091,26 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1408,640 +1417,612 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AZ46"/>
+  <dimension ref="A1:BA46"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AC3" sqref="A3:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="15.140625" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="23.42578125" customWidth="1"/>
-    <col min="14" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="37" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.42578125" customWidth="1"/>
-    <col min="39" max="48" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="49" max="51" width="13.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="24.1796875" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="15.1796875" customWidth="1"/>
+    <col min="13" max="13" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.453125" customWidth="1"/>
+    <col min="15" max="16" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="30" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="33" max="38" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.453125" customWidth="1"/>
+    <col min="40" max="49" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="50" max="52" width="13.453125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="18.75" customHeight="1">
+    <row r="1" spans="1:53" ht="18.75" customHeight="1">
       <c r="A1" t="s">
         <v>245</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="M1" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="X1" s="14" t="s">
+      <c r="N1" s="19"/>
+      <c r="Y1" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="AB1" s="14" t="s">
+      <c r="AC1" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="AE1" s="14" t="s">
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="AF1" s="14" t="s">
+      <c r="AI1" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="AO1" s="14" t="s">
+      <c r="AR1" s="18" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="2" spans="1:52" ht="18.75" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="AX1"/>
+      <c r="BA1" s="11"/>
+    </row>
+    <row r="2" spans="1:53" ht="18.75" customHeight="1">
+      <c r="A2" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="E2" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="G2" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>259</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="W2" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y2" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z2" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA2" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="AB2" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC2" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="AD2" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="AE2" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="AF2" s="21" t="s">
+        <v>278</v>
+      </c>
+      <c r="AG2" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="AH2" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="AI2" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="AJ2" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="AK2" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="AL2" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="AM2" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AN2" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="AO2" s="14" t="s">
         <v>271</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>259</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>276</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>277</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>278</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>279</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>274</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>272</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>262</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="Q2" s="12" t="s">
+      <c r="AP2" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="AQ2" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="AR2" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="AS2" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="AT2" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="AU2" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="AV2" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="AW2" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="AX2" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="AY2" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="R2" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="X2" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="Z2" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="AA2" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="AB2" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="AC2" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="AD2" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="AE2" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="AF2" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="AG2" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="AH2" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="AI2" s="12" t="s">
-        <v>236</v>
-      </c>
-      <c r="AJ2" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="AK2" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="AL2" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="AM2" s="17" t="s">
-        <v>242</v>
-      </c>
-      <c r="AN2" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="AO2" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="AP2" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="AQ2" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="AR2" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="AS2" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="AT2" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="AU2" s="12" t="s">
-        <v>244</v>
-      </c>
-      <c r="AW2" s="13" t="s">
+      <c r="AZ2" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="AX2" s="13" t="s">
+      <c r="BA2" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="AY2" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="AZ2" s="16" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="3" spans="1:52" ht="24" customHeight="1">
-      <c r="J3" s="22"/>
-      <c r="X3" s="14"/>
-      <c r="AD3" s="9"/>
-      <c r="AO3" s="14"/>
-      <c r="AW3" s="9"/>
-      <c r="AY3" s="9"/>
-    </row>
-    <row r="4" spans="1:52" ht="18.75" customHeight="1">
-      <c r="J4" s="22"/>
-      <c r="X4" s="14"/>
-      <c r="AD4" s="9"/>
-      <c r="AO4" s="14"/>
-      <c r="AW4" s="9"/>
-      <c r="AX4" s="10"/>
-      <c r="AY4" s="9"/>
-    </row>
-    <row r="5" spans="1:52" ht="18.75" customHeight="1">
-      <c r="J5" s="22"/>
-      <c r="X5" s="14"/>
-      <c r="AD5" s="9"/>
-      <c r="AO5" s="14"/>
-      <c r="AW5" s="9"/>
+    </row>
+    <row r="3" spans="1:53" ht="24" customHeight="1">
+      <c r="L3" s="17"/>
+      <c r="Y3" s="12"/>
+      <c r="AE3" s="9"/>
+      <c r="AP3" s="12"/>
+      <c r="AX3" s="9"/>
+      <c r="AZ3" s="9"/>
+    </row>
+    <row r="4" spans="1:53" ht="18.75" customHeight="1">
+      <c r="L4" s="17"/>
+      <c r="Y4" s="12"/>
+      <c r="AE4" s="9"/>
+      <c r="AP4" s="12"/>
+      <c r="AX4" s="9"/>
+      <c r="AY4" s="10"/>
+      <c r="AZ4" s="9"/>
+    </row>
+    <row r="5" spans="1:53" ht="18.75" customHeight="1">
+      <c r="L5" s="17"/>
+      <c r="Y5" s="12"/>
+      <c r="AE5" s="9"/>
+      <c r="AP5" s="12"/>
       <c r="AX5" s="9"/>
       <c r="AY5" s="9"/>
-    </row>
-    <row r="6" spans="1:52" ht="18.75" customHeight="1">
-      <c r="J6" s="22"/>
-      <c r="X6" s="14"/>
-      <c r="AD6" s="9"/>
-      <c r="AO6" s="14"/>
-      <c r="AW6" s="9"/>
-      <c r="AX6" s="10"/>
-      <c r="AY6" s="9"/>
-    </row>
-    <row r="7" spans="1:52" ht="18.75" customHeight="1">
-      <c r="J7" s="22"/>
-      <c r="X7" s="14"/>
-      <c r="AD7" s="9"/>
-      <c r="AO7" s="14"/>
-      <c r="AX7" s="10"/>
-      <c r="AY7" s="9"/>
-    </row>
-    <row r="8" spans="1:52" ht="18.75" customHeight="1">
-      <c r="X8" s="14"/>
-      <c r="AD8" s="9"/>
-      <c r="AO8" s="14"/>
-      <c r="AW8" s="9"/>
+      <c r="AZ5" s="9"/>
+    </row>
+    <row r="6" spans="1:53" ht="18.75" customHeight="1">
+      <c r="L6" s="17"/>
+      <c r="Y6" s="12"/>
+      <c r="AE6" s="9"/>
+      <c r="AP6" s="12"/>
+      <c r="AX6" s="9"/>
+      <c r="AY6" s="10"/>
+      <c r="AZ6" s="9"/>
+    </row>
+    <row r="7" spans="1:53" ht="18.75" customHeight="1">
+      <c r="L7" s="17"/>
+      <c r="Y7" s="12"/>
+      <c r="AE7" s="9"/>
+      <c r="AP7" s="12"/>
+      <c r="AY7" s="10"/>
+      <c r="AZ7" s="9"/>
+    </row>
+    <row r="8" spans="1:53" ht="18.75" customHeight="1">
+      <c r="Y8" s="12"/>
+      <c r="AE8" s="9"/>
+      <c r="AP8" s="12"/>
       <c r="AX8" s="9"/>
       <c r="AY8" s="9"/>
-    </row>
-    <row r="9" spans="1:52" ht="18.75" customHeight="1">
-      <c r="X9" s="14"/>
-      <c r="AD9" s="9"/>
-      <c r="AO9" s="14"/>
-    </row>
-    <row r="10" spans="1:52" ht="18.75" customHeight="1">
-      <c r="K10" s="14"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="X10" s="14"/>
-      <c r="AB10" s="14"/>
-      <c r="AE10" s="14"/>
-      <c r="AF10" s="14"/>
-      <c r="AO10" s="14"/>
-    </row>
-    <row r="11" spans="1:52" ht="18.75" customHeight="1">
-      <c r="K11" s="14"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="X11" s="14"/>
-      <c r="AB11" s="14"/>
-      <c r="AE11" s="14"/>
-      <c r="AF11" s="14"/>
-      <c r="AO11" s="14"/>
-    </row>
-    <row r="12" spans="1:52" ht="18.75" customHeight="1">
-      <c r="K12" s="14"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="X12" s="14"/>
-      <c r="AB12" s="14"/>
-      <c r="AE12" s="14"/>
-      <c r="AF12" s="14"/>
-      <c r="AO12" s="14"/>
-    </row>
-    <row r="13" spans="1:52" ht="18.75" customHeight="1">
-      <c r="K13" s="14"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="X13" s="14"/>
-      <c r="AB13" s="14"/>
-      <c r="AE13" s="14"/>
-      <c r="AF13" s="14"/>
-      <c r="AO13" s="14"/>
-    </row>
-    <row r="14" spans="1:52" ht="18.75" customHeight="1">
-      <c r="K14" s="14"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="X14" s="14"/>
-      <c r="AB14" s="14"/>
-      <c r="AE14" s="14"/>
-      <c r="AF14" s="14"/>
-      <c r="AO14" s="14"/>
-    </row>
-    <row r="15" spans="1:52" ht="18.75" customHeight="1">
-      <c r="K15" s="14"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="X15" s="14"/>
-      <c r="AB15" s="14"/>
-      <c r="AE15" s="14"/>
-      <c r="AF15" s="14"/>
-      <c r="AO15" s="14"/>
-    </row>
-    <row r="16" spans="1:52" ht="18.75" customHeight="1">
-      <c r="K16" s="14"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="X16" s="14"/>
-      <c r="AB16" s="14"/>
-      <c r="AE16" s="14"/>
-      <c r="AF16" s="14"/>
-      <c r="AO16" s="14"/>
-    </row>
-    <row r="17" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K17" s="14"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="X17" s="14"/>
-      <c r="AB17" s="14"/>
-      <c r="AE17" s="14"/>
-      <c r="AF17" s="14"/>
-      <c r="AO17" s="14"/>
-    </row>
-    <row r="18" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K18" s="14"/>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="X18" s="14"/>
-      <c r="AB18" s="14"/>
-      <c r="AE18" s="14"/>
-      <c r="AF18" s="14"/>
-      <c r="AO18" s="14"/>
-    </row>
-    <row r="19" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K19" s="14"/>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="X19" s="14"/>
-      <c r="AB19" s="14"/>
-      <c r="AE19" s="14"/>
-      <c r="AF19" s="14"/>
-      <c r="AO19" s="14"/>
-    </row>
-    <row r="20" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K20" s="14"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="X20" s="14"/>
-      <c r="AB20" s="14"/>
-      <c r="AE20" s="14"/>
-      <c r="AF20" s="14"/>
-      <c r="AO20" s="14"/>
-    </row>
-    <row r="21" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K21" s="14"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="X21" s="14"/>
-      <c r="AB21" s="14"/>
-      <c r="AE21" s="14"/>
-      <c r="AF21" s="14"/>
-      <c r="AO21" s="14"/>
-    </row>
-    <row r="22" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K22" s="14"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="X22" s="14"/>
-      <c r="AB22" s="14"/>
-      <c r="AE22" s="14"/>
-      <c r="AF22" s="14"/>
-      <c r="AO22" s="14"/>
-    </row>
-    <row r="23" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K23" s="14"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="X23" s="14"/>
-      <c r="AB23" s="14"/>
-      <c r="AE23" s="14"/>
-      <c r="AF23" s="14"/>
-      <c r="AO23" s="14"/>
-    </row>
-    <row r="24" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K24" s="14"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="X24" s="14"/>
-      <c r="AB24" s="14"/>
-      <c r="AE24" s="14"/>
-      <c r="AF24" s="14"/>
-      <c r="AO24" s="14"/>
-    </row>
-    <row r="25" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K25" s="14"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="X25" s="14"/>
-      <c r="AB25" s="14"/>
-      <c r="AE25" s="14"/>
-      <c r="AF25" s="14"/>
-      <c r="AO25" s="14"/>
-    </row>
-    <row r="26" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K26" s="14"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="X26" s="14"/>
-      <c r="AB26" s="14"/>
-      <c r="AE26" s="14"/>
-      <c r="AF26" s="14"/>
-      <c r="AO26" s="14"/>
-    </row>
-    <row r="27" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K27" s="14"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="X27" s="14"/>
-      <c r="AB27" s="14"/>
-      <c r="AE27" s="14"/>
-      <c r="AF27" s="14"/>
-      <c r="AO27" s="14"/>
-    </row>
-    <row r="28" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K28" s="14"/>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="X28" s="14"/>
-      <c r="AB28" s="14"/>
-      <c r="AE28" s="14"/>
-      <c r="AF28" s="14"/>
-      <c r="AO28" s="14"/>
-    </row>
-    <row r="29" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K29" s="14"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="X29" s="14"/>
-      <c r="AB29" s="14"/>
-      <c r="AE29" s="14"/>
-      <c r="AF29" s="14"/>
-      <c r="AO29" s="14"/>
-    </row>
-    <row r="30" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K30" s="14"/>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="X30" s="14"/>
-      <c r="AB30" s="14"/>
-      <c r="AE30" s="14"/>
-      <c r="AF30" s="14"/>
-      <c r="AO30" s="14"/>
-    </row>
-    <row r="31" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K31" s="14"/>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="X31" s="14"/>
-      <c r="AB31" s="14"/>
-      <c r="AE31" s="14"/>
-      <c r="AF31" s="14"/>
-      <c r="AO31" s="14"/>
-    </row>
-    <row r="32" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K32" s="14"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="X32" s="14"/>
-      <c r="AB32" s="14"/>
-      <c r="AE32" s="14"/>
-      <c r="AF32" s="14"/>
-      <c r="AO32" s="14"/>
-    </row>
-    <row r="33" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K33" s="14"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="X33" s="14"/>
-      <c r="AB33" s="14"/>
-      <c r="AE33" s="14"/>
-      <c r="AF33" s="14"/>
-      <c r="AO33" s="14"/>
-    </row>
-    <row r="34" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K34" s="14"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="X34" s="14"/>
-      <c r="AB34" s="14"/>
-      <c r="AE34" s="14"/>
-      <c r="AF34" s="14"/>
-      <c r="AO34" s="14"/>
-    </row>
-    <row r="35" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K35" s="14"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="X35" s="14"/>
-      <c r="AB35" s="14"/>
-      <c r="AE35" s="14"/>
-      <c r="AF35" s="14"/>
-      <c r="AO35" s="14"/>
-    </row>
-    <row r="36" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K36" s="14"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="X36" s="14"/>
-      <c r="AB36" s="14"/>
-      <c r="AE36" s="14"/>
-      <c r="AF36" s="14"/>
-      <c r="AO36" s="14"/>
-    </row>
-    <row r="37" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K37" s="14"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="X37" s="14"/>
-      <c r="AB37" s="14"/>
-      <c r="AE37" s="14"/>
-      <c r="AF37" s="14"/>
-      <c r="AO37" s="14"/>
-    </row>
-    <row r="38" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K38" s="14"/>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="X38" s="14"/>
-      <c r="AB38" s="14"/>
-      <c r="AE38" s="14"/>
-      <c r="AF38" s="14"/>
-      <c r="AO38" s="14"/>
-    </row>
-    <row r="39" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K39" s="14"/>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="X39" s="14"/>
-      <c r="AB39" s="14"/>
-      <c r="AE39" s="14"/>
-      <c r="AF39" s="14"/>
-      <c r="AO39" s="14"/>
-    </row>
-    <row r="40" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K40" s="14"/>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="X40" s="14"/>
-      <c r="AB40" s="14"/>
-      <c r="AE40" s="14"/>
-      <c r="AF40" s="14"/>
-      <c r="AO40" s="14"/>
-    </row>
-    <row r="41" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K41" s="14"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="X41" s="14"/>
-      <c r="AB41" s="14"/>
-      <c r="AE41" s="14"/>
-      <c r="AF41" s="14"/>
-      <c r="AO41" s="14"/>
-    </row>
-    <row r="42" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K42" s="14"/>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="X42" s="14"/>
-      <c r="AB42" s="14"/>
-      <c r="AE42" s="14"/>
-      <c r="AF42" s="14"/>
-      <c r="AO42" s="14"/>
-    </row>
-    <row r="43" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K43" s="14"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="X43" s="14"/>
-      <c r="AB43" s="14"/>
-      <c r="AE43" s="14"/>
-      <c r="AF43" s="14"/>
-      <c r="AO43" s="14"/>
-    </row>
-    <row r="44" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K44" s="14"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="X44" s="14"/>
-      <c r="AB44" s="14"/>
-      <c r="AE44" s="14"/>
-      <c r="AF44" s="14"/>
-      <c r="AO44" s="14"/>
-    </row>
-    <row r="45" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K45" s="14"/>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="X45" s="14"/>
-      <c r="AB45" s="14"/>
-      <c r="AE45" s="14"/>
-      <c r="AF45" s="14"/>
-      <c r="AO45" s="14"/>
-    </row>
-    <row r="46" spans="11:41" ht="18.75" customHeight="1">
-      <c r="K46" s="14"/>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="X46" s="14"/>
-      <c r="AB46" s="14"/>
-      <c r="AE46" s="14"/>
-      <c r="AF46" s="14"/>
-      <c r="AO46" s="14"/>
+      <c r="AZ8" s="9"/>
+    </row>
+    <row r="9" spans="1:53" ht="18.75" customHeight="1">
+      <c r="Y9" s="12"/>
+      <c r="AE9" s="9"/>
+      <c r="AP9" s="12"/>
+    </row>
+    <row r="10" spans="1:53" ht="18.75" customHeight="1">
+      <c r="M10" s="12"/>
+      <c r="N10" s="15"/>
+      <c r="Y10" s="12"/>
+      <c r="AC10" s="12"/>
+      <c r="AF10" s="12"/>
+      <c r="AG10" s="12"/>
+      <c r="AP10" s="12"/>
+    </row>
+    <row r="11" spans="1:53" ht="18.75" customHeight="1">
+      <c r="M11" s="12"/>
+      <c r="N11" s="15"/>
+      <c r="Y11" s="12"/>
+      <c r="AC11" s="12"/>
+      <c r="AF11" s="12"/>
+      <c r="AG11" s="12"/>
+      <c r="AP11" s="12"/>
+    </row>
+    <row r="12" spans="1:53" ht="18.75" customHeight="1">
+      <c r="M12" s="12"/>
+      <c r="N12" s="15"/>
+      <c r="Y12" s="12"/>
+      <c r="AC12" s="12"/>
+      <c r="AF12" s="12"/>
+      <c r="AG12" s="12"/>
+      <c r="AP12" s="12"/>
+    </row>
+    <row r="13" spans="1:53" ht="18.75" customHeight="1">
+      <c r="M13" s="12"/>
+      <c r="N13" s="15"/>
+      <c r="Y13" s="12"/>
+      <c r="AC13" s="12"/>
+      <c r="AF13" s="12"/>
+      <c r="AG13" s="12"/>
+      <c r="AP13" s="12"/>
+    </row>
+    <row r="14" spans="1:53" ht="18.75" customHeight="1">
+      <c r="M14" s="12"/>
+      <c r="N14" s="15"/>
+      <c r="Y14" s="12"/>
+      <c r="AC14" s="12"/>
+      <c r="AF14" s="12"/>
+      <c r="AG14" s="12"/>
+      <c r="AP14" s="12"/>
+    </row>
+    <row r="15" spans="1:53" ht="18.75" customHeight="1">
+      <c r="M15" s="12"/>
+      <c r="N15" s="15"/>
+      <c r="Y15" s="12"/>
+      <c r="AC15" s="12"/>
+      <c r="AF15" s="12"/>
+      <c r="AG15" s="12"/>
+      <c r="AP15" s="12"/>
+    </row>
+    <row r="16" spans="1:53" ht="18.75" customHeight="1">
+      <c r="M16" s="12"/>
+      <c r="N16" s="15"/>
+      <c r="Y16" s="12"/>
+      <c r="AC16" s="12"/>
+      <c r="AF16" s="12"/>
+      <c r="AG16" s="12"/>
+      <c r="AP16" s="12"/>
+    </row>
+    <row r="17" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M17" s="12"/>
+      <c r="N17" s="15"/>
+      <c r="Y17" s="12"/>
+      <c r="AC17" s="12"/>
+      <c r="AF17" s="12"/>
+      <c r="AG17" s="12"/>
+      <c r="AP17" s="12"/>
+    </row>
+    <row r="18" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M18" s="12"/>
+      <c r="N18" s="15"/>
+      <c r="Y18" s="12"/>
+      <c r="AC18" s="12"/>
+      <c r="AF18" s="12"/>
+      <c r="AG18" s="12"/>
+      <c r="AP18" s="12"/>
+    </row>
+    <row r="19" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M19" s="12"/>
+      <c r="N19" s="15"/>
+      <c r="Y19" s="12"/>
+      <c r="AC19" s="12"/>
+      <c r="AF19" s="12"/>
+      <c r="AG19" s="12"/>
+      <c r="AP19" s="12"/>
+    </row>
+    <row r="20" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M20" s="12"/>
+      <c r="N20" s="15"/>
+      <c r="Y20" s="12"/>
+      <c r="AC20" s="12"/>
+      <c r="AF20" s="12"/>
+      <c r="AG20" s="12"/>
+      <c r="AP20" s="12"/>
+    </row>
+    <row r="21" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M21" s="12"/>
+      <c r="N21" s="15"/>
+      <c r="Y21" s="12"/>
+      <c r="AC21" s="12"/>
+      <c r="AF21" s="12"/>
+      <c r="AG21" s="12"/>
+      <c r="AP21" s="12"/>
+    </row>
+    <row r="22" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M22" s="12"/>
+      <c r="N22" s="15"/>
+      <c r="Y22" s="12"/>
+      <c r="AC22" s="12"/>
+      <c r="AF22" s="12"/>
+      <c r="AG22" s="12"/>
+      <c r="AP22" s="12"/>
+    </row>
+    <row r="23" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M23" s="12"/>
+      <c r="N23" s="15"/>
+      <c r="Y23" s="12"/>
+      <c r="AC23" s="12"/>
+      <c r="AF23" s="12"/>
+      <c r="AG23" s="12"/>
+      <c r="AP23" s="12"/>
+    </row>
+    <row r="24" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M24" s="12"/>
+      <c r="N24" s="15"/>
+      <c r="Y24" s="12"/>
+      <c r="AC24" s="12"/>
+      <c r="AF24" s="12"/>
+      <c r="AG24" s="12"/>
+      <c r="AP24" s="12"/>
+    </row>
+    <row r="25" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M25" s="12"/>
+      <c r="N25" s="15"/>
+      <c r="Y25" s="12"/>
+      <c r="AC25" s="12"/>
+      <c r="AF25" s="12"/>
+      <c r="AG25" s="12"/>
+      <c r="AP25" s="12"/>
+    </row>
+    <row r="26" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M26" s="12"/>
+      <c r="N26" s="15"/>
+      <c r="Y26" s="12"/>
+      <c r="AC26" s="12"/>
+      <c r="AF26" s="12"/>
+      <c r="AG26" s="12"/>
+      <c r="AP26" s="12"/>
+    </row>
+    <row r="27" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M27" s="12"/>
+      <c r="N27" s="15"/>
+      <c r="Y27" s="12"/>
+      <c r="AC27" s="12"/>
+      <c r="AF27" s="12"/>
+      <c r="AG27" s="12"/>
+      <c r="AP27" s="12"/>
+    </row>
+    <row r="28" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M28" s="12"/>
+      <c r="N28" s="15"/>
+      <c r="Y28" s="12"/>
+      <c r="AC28" s="12"/>
+      <c r="AF28" s="12"/>
+      <c r="AG28" s="12"/>
+      <c r="AP28" s="12"/>
+    </row>
+    <row r="29" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M29" s="12"/>
+      <c r="N29" s="15"/>
+      <c r="Y29" s="12"/>
+      <c r="AC29" s="12"/>
+      <c r="AF29" s="12"/>
+      <c r="AG29" s="12"/>
+      <c r="AP29" s="12"/>
+    </row>
+    <row r="30" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M30" s="12"/>
+      <c r="N30" s="15"/>
+      <c r="Y30" s="12"/>
+      <c r="AC30" s="12"/>
+      <c r="AF30" s="12"/>
+      <c r="AG30" s="12"/>
+      <c r="AP30" s="12"/>
+    </row>
+    <row r="31" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M31" s="12"/>
+      <c r="N31" s="15"/>
+      <c r="Y31" s="12"/>
+      <c r="AC31" s="12"/>
+      <c r="AF31" s="12"/>
+      <c r="AG31" s="12"/>
+      <c r="AP31" s="12"/>
+    </row>
+    <row r="32" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M32" s="12"/>
+      <c r="N32" s="15"/>
+      <c r="Y32" s="12"/>
+      <c r="AC32" s="12"/>
+      <c r="AF32" s="12"/>
+      <c r="AG32" s="12"/>
+      <c r="AP32" s="12"/>
+    </row>
+    <row r="33" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M33" s="12"/>
+      <c r="N33" s="15"/>
+      <c r="Y33" s="12"/>
+      <c r="AC33" s="12"/>
+      <c r="AF33" s="12"/>
+      <c r="AG33" s="12"/>
+      <c r="AP33" s="12"/>
+    </row>
+    <row r="34" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M34" s="12"/>
+      <c r="N34" s="15"/>
+      <c r="Y34" s="12"/>
+      <c r="AC34" s="12"/>
+      <c r="AF34" s="12"/>
+      <c r="AG34" s="12"/>
+      <c r="AP34" s="12"/>
+    </row>
+    <row r="35" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M35" s="12"/>
+      <c r="N35" s="15"/>
+      <c r="Y35" s="12"/>
+      <c r="AC35" s="12"/>
+      <c r="AF35" s="12"/>
+      <c r="AG35" s="12"/>
+      <c r="AP35" s="12"/>
+    </row>
+    <row r="36" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M36" s="12"/>
+      <c r="N36" s="15"/>
+      <c r="Y36" s="12"/>
+      <c r="AC36" s="12"/>
+      <c r="AF36" s="12"/>
+      <c r="AG36" s="12"/>
+      <c r="AP36" s="12"/>
+    </row>
+    <row r="37" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M37" s="12"/>
+      <c r="N37" s="15"/>
+      <c r="Y37" s="12"/>
+      <c r="AC37" s="12"/>
+      <c r="AF37" s="12"/>
+      <c r="AG37" s="12"/>
+      <c r="AP37" s="12"/>
+    </row>
+    <row r="38" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M38" s="12"/>
+      <c r="N38" s="15"/>
+      <c r="Y38" s="12"/>
+      <c r="AC38" s="12"/>
+      <c r="AF38" s="12"/>
+      <c r="AG38" s="12"/>
+      <c r="AP38" s="12"/>
+    </row>
+    <row r="39" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M39" s="12"/>
+      <c r="N39" s="15"/>
+      <c r="Y39" s="12"/>
+      <c r="AC39" s="12"/>
+      <c r="AF39" s="12"/>
+      <c r="AG39" s="12"/>
+      <c r="AP39" s="12"/>
+    </row>
+    <row r="40" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M40" s="12"/>
+      <c r="N40" s="15"/>
+      <c r="Y40" s="12"/>
+      <c r="AC40" s="12"/>
+      <c r="AF40" s="12"/>
+      <c r="AG40" s="12"/>
+      <c r="AP40" s="12"/>
+    </row>
+    <row r="41" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M41" s="12"/>
+      <c r="N41" s="15"/>
+      <c r="Y41" s="12"/>
+      <c r="AC41" s="12"/>
+      <c r="AF41" s="12"/>
+      <c r="AG41" s="12"/>
+      <c r="AP41" s="12"/>
+    </row>
+    <row r="42" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M42" s="12"/>
+      <c r="N42" s="15"/>
+      <c r="Y42" s="12"/>
+      <c r="AC42" s="12"/>
+      <c r="AF42" s="12"/>
+      <c r="AG42" s="12"/>
+      <c r="AP42" s="12"/>
+    </row>
+    <row r="43" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M43" s="12"/>
+      <c r="N43" s="15"/>
+      <c r="Y43" s="12"/>
+      <c r="AC43" s="12"/>
+      <c r="AF43" s="12"/>
+      <c r="AG43" s="12"/>
+      <c r="AP43" s="12"/>
+    </row>
+    <row r="44" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M44" s="12"/>
+      <c r="N44" s="15"/>
+      <c r="Y44" s="12"/>
+      <c r="AC44" s="12"/>
+      <c r="AF44" s="12"/>
+      <c r="AG44" s="12"/>
+      <c r="AP44" s="12"/>
+    </row>
+    <row r="45" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M45" s="12"/>
+      <c r="N45" s="15"/>
+      <c r="Y45" s="12"/>
+      <c r="AC45" s="12"/>
+      <c r="AF45" s="12"/>
+      <c r="AG45" s="12"/>
+      <c r="AP45" s="12"/>
+    </row>
+    <row r="46" spans="13:42" ht="18.75" customHeight="1">
+      <c r="M46" s="12"/>
+      <c r="N46" s="15"/>
+      <c r="Y46" s="12"/>
+      <c r="AC46" s="12"/>
+      <c r="AF46" s="12"/>
+      <c r="AG46" s="12"/>
+      <c r="AP46" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2056,27 +2037,27 @@
   </sheetPr>
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0"/>
+    <sheetView topLeftCell="A89" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2090,10 +2071,10 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="21"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -2107,10 +2088,10 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -2124,10 +2105,10 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -2141,10 +2122,10 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="20"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -2158,10 +2139,10 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2175,10 +2156,10 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -2192,10 +2173,10 @@
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="20"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -2209,10 +2190,10 @@
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="20"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -2226,10 +2207,10 @@
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -2243,10 +2224,10 @@
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="20"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -2260,10 +2241,10 @@
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -2277,10 +2258,10 @@
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="20"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2294,10 +2275,10 @@
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -2311,10 +2292,10 @@
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="20"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -2328,10 +2309,10 @@
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="20"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -2345,10 +2326,10 @@
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="20"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -2362,10 +2343,10 @@
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="20"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -2379,10 +2360,10 @@
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="20"/>
+      <c r="C19" s="22"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -2396,10 +2377,10 @@
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="20"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -2413,10 +2394,10 @@
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="20"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -2430,10 +2411,10 @@
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="20"/>
+      <c r="C22" s="22"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -2447,10 +2428,10 @@
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="20"/>
+      <c r="C23" s="22"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -2464,10 +2445,10 @@
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="20"/>
+      <c r="C24" s="22"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -2677,10 +2658,10 @@
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="20"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -2692,8 +2673,8 @@
     </row>
     <row r="38" spans="1:11" ht="18.75" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -2707,10 +2688,10 @@
       <c r="A39" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="21"/>
+      <c r="C39" s="23"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -2724,10 +2705,10 @@
       <c r="A40" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="20"/>
+      <c r="C40" s="22"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -2741,10 +2722,10 @@
       <c r="A41" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="20"/>
+      <c r="C41" s="22"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -2758,10 +2739,10 @@
       <c r="A42" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="20"/>
+      <c r="C42" s="22"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -2775,10 +2756,10 @@
       <c r="A43" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="20"/>
+      <c r="C43" s="22"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -2792,10 +2773,10 @@
       <c r="A44" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="20"/>
+      <c r="C44" s="22"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2809,10 +2790,10 @@
       <c r="A45" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C45" s="20"/>
+      <c r="C45" s="22"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -2856,10 +2837,10 @@
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="20"/>
+      <c r="C48" s="22"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2871,8 +2852,8 @@
     </row>
     <row r="49" spans="1:11" ht="18.75" customHeight="1">
       <c r="A49" s="1"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -2886,10 +2867,10 @@
       <c r="A50" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B50" s="20" t="s">
+      <c r="B50" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="20"/>
+      <c r="C50" s="22"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
@@ -2903,10 +2884,10 @@
       <c r="A51" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C51" s="20"/>
+      <c r="C51" s="22"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -2920,10 +2901,10 @@
       <c r="A52" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="20"/>
+      <c r="C52" s="22"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2937,10 +2918,10 @@
       <c r="A53" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="C53" s="20"/>
+      <c r="C53" s="22"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -2954,10 +2935,10 @@
       <c r="A54" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="C54" s="20"/>
+      <c r="C54" s="22"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -2971,10 +2952,10 @@
       <c r="A55" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C55" s="20"/>
+      <c r="C55" s="22"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -2988,10 +2969,10 @@
       <c r="A56" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B56" s="20" t="s">
+      <c r="B56" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="C56" s="20"/>
+      <c r="C56" s="22"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
@@ -3005,10 +2986,10 @@
       <c r="A57" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="C57" s="20"/>
+      <c r="C57" s="22"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -3022,10 +3003,10 @@
       <c r="A58" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="C58" s="20"/>
+      <c r="C58" s="22"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
@@ -3039,10 +3020,10 @@
       <c r="A59" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="20"/>
+      <c r="C59" s="22"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
@@ -3056,10 +3037,10 @@
       <c r="A60" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="C60" s="20"/>
+      <c r="C60" s="22"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
@@ -3073,10 +3054,10 @@
       <c r="A61" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="C61" s="20"/>
+      <c r="C61" s="22"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
@@ -3090,10 +3071,10 @@
       <c r="A62" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="C62" s="20"/>
+      <c r="C62" s="22"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
@@ -3107,10 +3088,10 @@
       <c r="A63" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B63" s="20" t="s">
+      <c r="B63" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="C63" s="20"/>
+      <c r="C63" s="22"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
@@ -3124,10 +3105,10 @@
       <c r="A64" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B64" s="20" t="s">
+      <c r="B64" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="C64" s="20"/>
+      <c r="C64" s="22"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
@@ -3141,10 +3122,10 @@
       <c r="A65" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B65" s="20" t="s">
+      <c r="B65" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="C65" s="20"/>
+      <c r="C65" s="22"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
@@ -3158,10 +3139,10 @@
       <c r="A66" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B66" s="20" t="s">
+      <c r="B66" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C66" s="20"/>
+      <c r="C66" s="22"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
@@ -3175,10 +3156,10 @@
       <c r="A67" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="20"/>
+      <c r="C67" s="22"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
@@ -3192,10 +3173,10 @@
       <c r="A68" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B68" s="20" t="s">
+      <c r="B68" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="C68" s="20"/>
+      <c r="C68" s="22"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
@@ -3209,10 +3190,10 @@
       <c r="A69" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="C69" s="20"/>
+      <c r="C69" s="22"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
@@ -3226,10 +3207,10 @@
       <c r="A70" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B70" s="20" t="s">
+      <c r="B70" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="C70" s="20"/>
+      <c r="C70" s="22"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
@@ -3243,10 +3224,10 @@
       <c r="A71" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="C71" s="20"/>
+      <c r="C71" s="22"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
@@ -3260,10 +3241,10 @@
       <c r="A72" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="C72" s="20"/>
+      <c r="C72" s="22"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
@@ -3277,10 +3258,10 @@
       <c r="A73" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B73" s="20" t="s">
+      <c r="B73" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="C73" s="20"/>
+      <c r="C73" s="22"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
@@ -3294,10 +3275,10 @@
       <c r="A74" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B74" s="20" t="s">
+      <c r="B74" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="C74" s="20"/>
+      <c r="C74" s="22"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
@@ -3311,10 +3292,10 @@
       <c r="A75" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B75" s="20" t="s">
+      <c r="B75" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="C75" s="20"/>
+      <c r="C75" s="22"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
@@ -3328,10 +3309,10 @@
       <c r="A76" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B76" s="20" t="s">
+      <c r="B76" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="C76" s="20"/>
+      <c r="C76" s="22"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
@@ -3345,10 +3326,10 @@
       <c r="A77" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B77" s="20" t="s">
+      <c r="B77" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="C77" s="20"/>
+      <c r="C77" s="22"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
@@ -3936,61 +3917,6 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="B77:C77"/>
@@ -3999,6 +3925,61 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
change sex to host_sex and age to host_age in metadata_template.xlsx
</commit_message>
<xml_diff>
--- a/assets/metadata_template.xlsx
+++ b/assets/metadata_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\sample_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\01.scripts\tostadas\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149D3522-952C-4D1B-B7A1-0870DD324B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFEC4DF-D5AD-4180-83D5-4D6386254C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -705,12 +705,6 @@
     <t>ncbi_sequence_name_sra</t>
   </si>
   <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
     <t>state</t>
   </si>
   <si>
@@ -880,6 +874,12 @@
   </si>
   <si>
     <t>authors</t>
+  </si>
+  <si>
+    <t>host_sex</t>
+  </si>
+  <si>
+    <t>host_age</t>
   </si>
 </sst>
 </file>
@@ -1419,8 +1419,8 @@
   </sheetPr>
   <dimension ref="A1:BA46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -1448,191 +1448,191 @@
   <sheetData>
     <row r="1" spans="1:53" ht="18.75" customHeight="1">
       <c r="A1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="N1" s="19"/>
       <c r="Y1" s="18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="AC1" s="18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="AF1" s="11"/>
       <c r="AG1" s="11"/>
       <c r="AH1" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="AI1" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="AR1" s="18" t="s">
         <v>249</v>
-      </c>
-      <c r="AI1" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="AR1" s="18" t="s">
-        <v>251</v>
       </c>
       <c r="AX1"/>
       <c r="BA1" s="11"/>
     </row>
     <row r="2" spans="1:53" ht="18.75" customHeight="1">
       <c r="A2" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="O2" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="P2" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="W2" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="Y2" s="20" t="s">
         <v>280</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="G2" s="14" t="s">
+      <c r="Z2" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>273</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>274</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>275</v>
-      </c>
-      <c r="K2" s="16" t="s">
+      <c r="AA2" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AB2" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC2" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="AD2" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="AE2" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="AF2" s="21" t="s">
         <v>276</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="AG2" s="21" t="s">
         <v>277</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>259</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>272</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="U2" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="V2" s="14" t="s">
-        <v>232</v>
-      </c>
-      <c r="W2" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="X2" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="Y2" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z2" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="AA2" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="AB2" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="AC2" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="AD2" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="AF2" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="AG2" s="21" t="s">
-        <v>279</v>
       </c>
       <c r="AH2" s="20" t="s">
         <v>222</v>
       </c>
       <c r="AI2" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="AJ2" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="AK2" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="AL2" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="AJ2" s="14" t="s">
+      <c r="AM2" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="AN2" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="AO2" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="AP2" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="AQ2" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="AR2" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="AS2" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="AK2" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="AL2" s="14" t="s">
-        <v>236</v>
-      </c>
-      <c r="AM2" s="14" t="s">
+      <c r="AT2" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="AN2" s="14" t="s">
+      <c r="AU2" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="AV2" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="AW2" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="AO2" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="AP2" s="14" t="s">
+      <c r="AX2" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="AQ2" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="AR2" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="AS2" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="AT2" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="AU2" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="AV2" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="AW2" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="AX2" s="14" t="s">
-        <v>244</v>
-      </c>
       <c r="AY2" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="AZ2" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="BA2" s="13" t="s">
         <v>264</v>
-      </c>
-      <c r="AZ2" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="BA2" s="13" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:53" ht="24" customHeight="1">
@@ -3917,6 +3917,61 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="B77:C77"/>
@@ -3925,61 +3980,6 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update metadata template to match test metadata sheets
</commit_message>
<xml_diff>
--- a/assets/metadata_template.xlsx
+++ b/assets/metadata_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ick4\Downloads\sample_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\01.scripts\tostadas\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149D3522-952C-4D1B-B7A1-0870DD324B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF82C42-CA98-4111-95EF-539BECCEA148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -705,12 +705,6 @@
     <t>ncbi_sequence_name_sra</t>
   </si>
   <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
     <t>state</t>
   </si>
   <si>
@@ -880,6 +874,12 @@
   </si>
   <si>
     <t>authors</t>
+  </si>
+  <si>
+    <t>host_sex</t>
+  </si>
+  <si>
+    <t>host_age</t>
   </si>
 </sst>
 </file>
@@ -1417,10 +1417,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:BA46"/>
+  <dimension ref="A1:BB45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -1446,252 +1446,254 @@
     <col min="50" max="52" width="13.453125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="18.75" customHeight="1">
+    <row r="1" spans="1:54" ht="18.75" customHeight="1">
       <c r="A1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="N1" s="19"/>
       <c r="Y1" s="18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="AC1" s="18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="AF1" s="11"/>
       <c r="AG1" s="11"/>
       <c r="AH1" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="AI1" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="AR1" s="18" t="s">
         <v>249</v>
-      </c>
-      <c r="AI1" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="AR1" s="18" t="s">
-        <v>251</v>
       </c>
       <c r="AX1"/>
       <c r="BA1" s="11"/>
     </row>
-    <row r="2" spans="1:53" ht="18.75" customHeight="1">
+    <row r="2" spans="1:54" ht="18.75" customHeight="1">
       <c r="A2" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>275</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="O2" s="16"/>
+      <c r="P2" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="D2" s="14" t="s">
+      <c r="Q2" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="W2" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="Y2" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="Z2" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="AA2" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="AB2" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AC2" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD2" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="AE2" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="AF2" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="AG2" s="21" t="s">
+        <v>276</v>
+      </c>
+      <c r="AH2" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="AI2" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="AJ2" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="AK2" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="AL2" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="AM2" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="AN2" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="AO2" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="AP2" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>270</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>273</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>274</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>275</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>276</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>277</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>259</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>272</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="Q2" s="14" t="s">
+      <c r="AQ2" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="AR2" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="AS2" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="AT2" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="AU2" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="AV2" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="AW2" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="AX2" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="AY2" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="AZ2" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="R2" s="14" t="s">
+      <c r="BA2" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="S2" s="14" t="s">
-        <v>233</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="U2" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="V2" s="14" t="s">
-        <v>232</v>
-      </c>
-      <c r="W2" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="X2" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="Y2" s="20" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z2" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="AA2" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="AB2" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="AC2" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="AD2" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="AF2" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="AG2" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="AH2" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="AI2" s="20" t="s">
-        <v>234</v>
-      </c>
-      <c r="AJ2" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="AK2" s="14" t="s">
-        <v>235</v>
-      </c>
-      <c r="AL2" s="14" t="s">
-        <v>236</v>
-      </c>
-      <c r="AM2" s="14" t="s">
-        <v>237</v>
-      </c>
-      <c r="AN2" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="AO2" s="14" t="s">
-        <v>271</v>
-      </c>
-      <c r="AP2" s="14" t="s">
-        <v>242</v>
-      </c>
-      <c r="AQ2" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="AR2" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="AS2" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="AT2" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="AU2" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="AV2" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="AW2" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="AX2" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="AY2" s="13" t="s">
+      <c r="BB2" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="AZ2" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="BA2" s="13" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="3" spans="1:53" ht="24" customHeight="1">
+    </row>
+    <row r="3" spans="1:54" ht="18.75" customHeight="1">
       <c r="L3" s="17"/>
       <c r="Y3" s="12"/>
       <c r="AE3" s="9"/>
       <c r="AP3" s="12"/>
       <c r="AX3" s="9"/>
+      <c r="AY3" s="10"/>
       <c r="AZ3" s="9"/>
     </row>
-    <row r="4" spans="1:53" ht="18.75" customHeight="1">
+    <row r="4" spans="1:54" ht="18.75" customHeight="1">
       <c r="L4" s="17"/>
       <c r="Y4" s="12"/>
       <c r="AE4" s="9"/>
       <c r="AP4" s="12"/>
       <c r="AX4" s="9"/>
-      <c r="AY4" s="10"/>
+      <c r="AY4" s="9"/>
       <c r="AZ4" s="9"/>
     </row>
-    <row r="5" spans="1:53" ht="18.75" customHeight="1">
+    <row r="5" spans="1:54" ht="18.75" customHeight="1">
       <c r="L5" s="17"/>
       <c r="Y5" s="12"/>
       <c r="AE5" s="9"/>
       <c r="AP5" s="12"/>
       <c r="AX5" s="9"/>
-      <c r="AY5" s="9"/>
+      <c r="AY5" s="10"/>
       <c r="AZ5" s="9"/>
     </row>
-    <row r="6" spans="1:53" ht="18.75" customHeight="1">
+    <row r="6" spans="1:54" ht="18.75" customHeight="1">
       <c r="L6" s="17"/>
       <c r="Y6" s="12"/>
       <c r="AE6" s="9"/>
       <c r="AP6" s="12"/>
-      <c r="AX6" s="9"/>
       <c r="AY6" s="10"/>
       <c r="AZ6" s="9"/>
     </row>
-    <row r="7" spans="1:53" ht="18.75" customHeight="1">
-      <c r="L7" s="17"/>
+    <row r="7" spans="1:54" ht="18.75" customHeight="1">
       <c r="Y7" s="12"/>
       <c r="AE7" s="9"/>
       <c r="AP7" s="12"/>
-      <c r="AY7" s="10"/>
+      <c r="AX7" s="9"/>
+      <c r="AY7" s="9"/>
       <c r="AZ7" s="9"/>
     </row>
-    <row r="8" spans="1:53" ht="18.75" customHeight="1">
+    <row r="8" spans="1:54" ht="18.75" customHeight="1">
       <c r="Y8" s="12"/>
       <c r="AE8" s="9"/>
       <c r="AP8" s="12"/>
-      <c r="AX8" s="9"/>
-      <c r="AY8" s="9"/>
-      <c r="AZ8" s="9"/>
-    </row>
-    <row r="9" spans="1:53" ht="18.75" customHeight="1">
+    </row>
+    <row r="9" spans="1:54" ht="18.75" customHeight="1">
+      <c r="M9" s="12"/>
+      <c r="N9" s="15"/>
       <c r="Y9" s="12"/>
-      <c r="AE9" s="9"/>
+      <c r="AC9" s="12"/>
+      <c r="AF9" s="12"/>
+      <c r="AG9" s="12"/>
       <c r="AP9" s="12"/>
     </row>
-    <row r="10" spans="1:53" ht="18.75" customHeight="1">
+    <row r="10" spans="1:54" ht="18.75" customHeight="1">
       <c r="M10" s="12"/>
       <c r="N10" s="15"/>
       <c r="Y10" s="12"/>
@@ -1700,7 +1702,7 @@
       <c r="AG10" s="12"/>
       <c r="AP10" s="12"/>
     </row>
-    <row r="11" spans="1:53" ht="18.75" customHeight="1">
+    <row r="11" spans="1:54" ht="18.75" customHeight="1">
       <c r="M11" s="12"/>
       <c r="N11" s="15"/>
       <c r="Y11" s="12"/>
@@ -1709,7 +1711,7 @@
       <c r="AG11" s="12"/>
       <c r="AP11" s="12"/>
     </row>
-    <row r="12" spans="1:53" ht="18.75" customHeight="1">
+    <row r="12" spans="1:54" ht="18.75" customHeight="1">
       <c r="M12" s="12"/>
       <c r="N12" s="15"/>
       <c r="Y12" s="12"/>
@@ -1718,7 +1720,7 @@
       <c r="AG12" s="12"/>
       <c r="AP12" s="12"/>
     </row>
-    <row r="13" spans="1:53" ht="18.75" customHeight="1">
+    <row r="13" spans="1:54" ht="18.75" customHeight="1">
       <c r="M13" s="12"/>
       <c r="N13" s="15"/>
       <c r="Y13" s="12"/>
@@ -1727,7 +1729,7 @@
       <c r="AG13" s="12"/>
       <c r="AP13" s="12"/>
     </row>
-    <row r="14" spans="1:53" ht="18.75" customHeight="1">
+    <row r="14" spans="1:54" ht="18.75" customHeight="1">
       <c r="M14" s="12"/>
       <c r="N14" s="15"/>
       <c r="Y14" s="12"/>
@@ -1736,7 +1738,7 @@
       <c r="AG14" s="12"/>
       <c r="AP14" s="12"/>
     </row>
-    <row r="15" spans="1:53" ht="18.75" customHeight="1">
+    <row r="15" spans="1:54" ht="18.75" customHeight="1">
       <c r="M15" s="12"/>
       <c r="N15" s="15"/>
       <c r="Y15" s="12"/>
@@ -1745,7 +1747,7 @@
       <c r="AG15" s="12"/>
       <c r="AP15" s="12"/>
     </row>
-    <row r="16" spans="1:53" ht="18.75" customHeight="1">
+    <row r="16" spans="1:54" ht="18.75" customHeight="1">
       <c r="M16" s="12"/>
       <c r="N16" s="15"/>
       <c r="Y16" s="12"/>
@@ -2014,15 +2016,6 @@
       <c r="AF45" s="12"/>
       <c r="AG45" s="12"/>
       <c r="AP45" s="12"/>
-    </row>
-    <row r="46" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M46" s="12"/>
-      <c r="N46" s="15"/>
-      <c r="Y46" s="12"/>
-      <c r="AC46" s="12"/>
-      <c r="AF46" s="12"/>
-      <c r="AG46" s="12"/>
-      <c r="AP46" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update Excel files to remove ncbi-namespace that's now in submission config file
</commit_message>
<xml_diff>
--- a/assets/metadata_template.xlsx
+++ b/assets/metadata_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\01.scripts\tostadas\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFEC4DF-D5AD-4180-83D5-4D6386254C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A178197B-E2C2-4BB5-9D08-347A021DA591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="640" yWindow="3720" windowWidth="28800" windowHeight="12760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata_template" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="283">
   <si>
     <t>Strategy</t>
   </si>
@@ -834,9 +834,6 @@
     <t>ncbi-spuid</t>
   </si>
   <si>
-    <t>ncbi-spuid_namespace</t>
-  </si>
-  <si>
     <t>ncbi-bioproject</t>
   </si>
   <si>
@@ -880,6 +877,12 @@
   </si>
   <si>
     <t>host_age</t>
+  </si>
+  <si>
+    <t>illumina_library_name</t>
+  </si>
+  <si>
+    <t>nanopore_library_name</t>
   </si>
 </sst>
 </file>
@@ -1417,64 +1420,67 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:BA46"/>
+  <dimension ref="A1:BB46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AV6" sqref="AV6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="24.1796875" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="15.1796875" customWidth="1"/>
-    <col min="13" max="13" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.453125" customWidth="1"/>
-    <col min="15" max="16" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="30" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="33" max="38" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.453125" customWidth="1"/>
-    <col min="40" max="49" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="50" max="52" width="13.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="24.1796875" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="15.1796875" customWidth="1"/>
+    <col min="12" max="12" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.453125" customWidth="1"/>
+    <col min="14" max="15" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="29" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="32" max="37" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.453125" customWidth="1"/>
+    <col min="39" max="39" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.453125" customWidth="1"/>
+    <col min="41" max="49" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.453125" customWidth="1"/>
+    <col min="51" max="53" width="13.453125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="18.75" customHeight="1">
+    <row r="1" spans="1:54" ht="18.75" customHeight="1">
       <c r="A1" t="s">
         <v>243</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="L1" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="N1" s="19"/>
-      <c r="Y1" s="18" t="s">
+      <c r="M1" s="19"/>
+      <c r="X1" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AB1" s="18" t="s">
         <v>246</v>
       </c>
+      <c r="AE1" s="11"/>
       <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
+      <c r="AG1" s="18" t="s">
+        <v>247</v>
+      </c>
       <c r="AH1" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="AI1" s="18" t="s">
         <v>248</v>
       </c>
       <c r="AR1" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="AX1"/>
-      <c r="BA1" s="11"/>
-    </row>
-    <row r="2" spans="1:53" ht="18.75" customHeight="1">
+      <c r="AY1"/>
+      <c r="BB1" s="11"/>
+    </row>
+    <row r="2" spans="1:54" ht="18.75" customHeight="1">
       <c r="A2" s="14" t="s">
         <v>256</v>
       </c>
@@ -1485,16 +1491,16 @@
         <v>266</v>
       </c>
       <c r="D2" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>279</v>
+      <c r="G2" s="16" t="s">
+        <v>270</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>271</v>
@@ -1508,95 +1514,95 @@
       <c r="K2" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="V2" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="W2" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="X2" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="Y2" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="Z2" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA2" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="AB2" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="AC2" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="AD2" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="AE2" s="21" t="s">
         <v>275</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>257</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>270</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>259</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="U2" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="V2" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="W2" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="X2" s="14" t="s">
-        <v>229</v>
-      </c>
-      <c r="Y2" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="Z2" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="AA2" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="AB2" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="AC2" s="20" t="s">
-        <v>227</v>
-      </c>
-      <c r="AD2" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>226</v>
       </c>
       <c r="AF2" s="21" t="s">
         <v>276</v>
       </c>
-      <c r="AG2" s="21" t="s">
-        <v>277</v>
+      <c r="AG2" s="20" t="s">
+        <v>222</v>
       </c>
       <c r="AH2" s="20" t="s">
-        <v>222</v>
-      </c>
-      <c r="AI2" s="20" t="s">
         <v>232</v>
       </c>
+      <c r="AI2" s="14" t="s">
+        <v>252</v>
+      </c>
       <c r="AJ2" s="14" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="AK2" s="14" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AL2" s="14" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="AM2" s="14" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="AN2" s="14" t="s">
-        <v>253</v>
+        <v>281</v>
       </c>
       <c r="AO2" s="14" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AP2" s="14" t="s">
         <v>240</v>
@@ -1623,405 +1629,408 @@
         <v>255</v>
       </c>
       <c r="AX2" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="AY2" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="AY2" s="13" t="s">
+      <c r="AZ2" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="AZ2" s="13" t="s">
+      <c r="BA2" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="BA2" s="13" t="s">
+      <c r="BB2" s="13" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:53" ht="24" customHeight="1">
-      <c r="L3" s="17"/>
-      <c r="Y3" s="12"/>
-      <c r="AE3" s="9"/>
+    <row r="3" spans="1:54" ht="24" customHeight="1">
+      <c r="K3" s="17"/>
+      <c r="X3" s="12"/>
+      <c r="AD3" s="9"/>
       <c r="AP3" s="12"/>
-      <c r="AX3" s="9"/>
-      <c r="AZ3" s="9"/>
-    </row>
-    <row r="4" spans="1:53" ht="18.75" customHeight="1">
-      <c r="L4" s="17"/>
-      <c r="Y4" s="12"/>
-      <c r="AE4" s="9"/>
+      <c r="AY3" s="9"/>
+      <c r="BA3" s="9"/>
+    </row>
+    <row r="4" spans="1:54" ht="18.75" customHeight="1">
+      <c r="K4" s="17"/>
+      <c r="X4" s="12"/>
+      <c r="AD4" s="9"/>
       <c r="AP4" s="12"/>
-      <c r="AX4" s="9"/>
-      <c r="AY4" s="10"/>
-      <c r="AZ4" s="9"/>
-    </row>
-    <row r="5" spans="1:53" ht="18.75" customHeight="1">
-      <c r="L5" s="17"/>
-      <c r="Y5" s="12"/>
-      <c r="AE5" s="9"/>
+      <c r="AY4" s="9"/>
+      <c r="AZ4" s="10"/>
+      <c r="BA4" s="9"/>
+    </row>
+    <row r="5" spans="1:54" ht="18.75" customHeight="1">
+      <c r="K5" s="17"/>
+      <c r="X5" s="12"/>
+      <c r="AD5" s="9"/>
       <c r="AP5" s="12"/>
-      <c r="AX5" s="9"/>
       <c r="AY5" s="9"/>
       <c r="AZ5" s="9"/>
-    </row>
-    <row r="6" spans="1:53" ht="18.75" customHeight="1">
-      <c r="L6" s="17"/>
-      <c r="Y6" s="12"/>
-      <c r="AE6" s="9"/>
+      <c r="BA5" s="9"/>
+    </row>
+    <row r="6" spans="1:54" ht="18.75" customHeight="1">
+      <c r="K6" s="17"/>
+      <c r="X6" s="12"/>
+      <c r="AD6" s="9"/>
       <c r="AP6" s="12"/>
-      <c r="AX6" s="9"/>
-      <c r="AY6" s="10"/>
-      <c r="AZ6" s="9"/>
-    </row>
-    <row r="7" spans="1:53" ht="18.75" customHeight="1">
-      <c r="L7" s="17"/>
-      <c r="Y7" s="12"/>
-      <c r="AE7" s="9"/>
+      <c r="AY6" s="9"/>
+      <c r="AZ6" s="10"/>
+      <c r="BA6" s="9"/>
+    </row>
+    <row r="7" spans="1:54" ht="18.75" customHeight="1">
+      <c r="K7" s="17"/>
+      <c r="X7" s="12"/>
+      <c r="AD7" s="9"/>
       <c r="AP7" s="12"/>
-      <c r="AY7" s="10"/>
-      <c r="AZ7" s="9"/>
-    </row>
-    <row r="8" spans="1:53" ht="18.75" customHeight="1">
-      <c r="Y8" s="12"/>
-      <c r="AE8" s="9"/>
+      <c r="AZ7" s="10"/>
+      <c r="BA7" s="9"/>
+    </row>
+    <row r="8" spans="1:54" ht="18.75" customHeight="1">
+      <c r="X8" s="12"/>
+      <c r="AD8" s="9"/>
       <c r="AP8" s="12"/>
-      <c r="AX8" s="9"/>
       <c r="AY8" s="9"/>
       <c r="AZ8" s="9"/>
-    </row>
-    <row r="9" spans="1:53" ht="18.75" customHeight="1">
-      <c r="Y9" s="12"/>
-      <c r="AE9" s="9"/>
+      <c r="BA8" s="9"/>
+    </row>
+    <row r="9" spans="1:54" ht="18.75" customHeight="1">
+      <c r="X9" s="12"/>
+      <c r="AD9" s="9"/>
       <c r="AP9" s="12"/>
     </row>
-    <row r="10" spans="1:53" ht="18.75" customHeight="1">
-      <c r="M10" s="12"/>
-      <c r="N10" s="15"/>
-      <c r="Y10" s="12"/>
-      <c r="AC10" s="12"/>
+    <row r="10" spans="1:54" ht="18.75" customHeight="1">
+      <c r="L10" s="12"/>
+      <c r="M10" s="15"/>
+      <c r="X10" s="12"/>
+      <c r="AB10" s="12"/>
+      <c r="AE10" s="12"/>
       <c r="AF10" s="12"/>
-      <c r="AG10" s="12"/>
       <c r="AP10" s="12"/>
     </row>
-    <row r="11" spans="1:53" ht="18.75" customHeight="1">
-      <c r="M11" s="12"/>
-      <c r="N11" s="15"/>
-      <c r="Y11" s="12"/>
-      <c r="AC11" s="12"/>
+    <row r="11" spans="1:54" ht="18.75" customHeight="1">
+      <c r="L11" s="12"/>
+      <c r="M11" s="15"/>
+      <c r="X11" s="12"/>
+      <c r="AB11" s="12"/>
+      <c r="AE11" s="12"/>
       <c r="AF11" s="12"/>
-      <c r="AG11" s="12"/>
       <c r="AP11" s="12"/>
     </row>
-    <row r="12" spans="1:53" ht="18.75" customHeight="1">
-      <c r="M12" s="12"/>
-      <c r="N12" s="15"/>
-      <c r="Y12" s="12"/>
-      <c r="AC12" s="12"/>
+    <row r="12" spans="1:54" ht="18.75" customHeight="1">
+      <c r="L12" s="12"/>
+      <c r="M12" s="15"/>
+      <c r="X12" s="12"/>
+      <c r="AB12" s="12"/>
+      <c r="AE12" s="12"/>
       <c r="AF12" s="12"/>
-      <c r="AG12" s="12"/>
       <c r="AP12" s="12"/>
     </row>
-    <row r="13" spans="1:53" ht="18.75" customHeight="1">
-      <c r="M13" s="12"/>
-      <c r="N13" s="15"/>
-      <c r="Y13" s="12"/>
-      <c r="AC13" s="12"/>
+    <row r="13" spans="1:54" ht="18.75" customHeight="1">
+      <c r="L13" s="12"/>
+      <c r="M13" s="15"/>
+      <c r="X13" s="12"/>
+      <c r="AB13" s="12"/>
+      <c r="AE13" s="12"/>
       <c r="AF13" s="12"/>
-      <c r="AG13" s="12"/>
       <c r="AP13" s="12"/>
     </row>
-    <row r="14" spans="1:53" ht="18.75" customHeight="1">
-      <c r="M14" s="12"/>
-      <c r="N14" s="15"/>
-      <c r="Y14" s="12"/>
-      <c r="AC14" s="12"/>
+    <row r="14" spans="1:54" ht="18.75" customHeight="1">
+      <c r="L14" s="12"/>
+      <c r="M14" s="15"/>
+      <c r="X14" s="12"/>
+      <c r="AB14" s="12"/>
+      <c r="AE14" s="12"/>
       <c r="AF14" s="12"/>
-      <c r="AG14" s="12"/>
       <c r="AP14" s="12"/>
     </row>
-    <row r="15" spans="1:53" ht="18.75" customHeight="1">
-      <c r="M15" s="12"/>
-      <c r="N15" s="15"/>
-      <c r="Y15" s="12"/>
-      <c r="AC15" s="12"/>
+    <row r="15" spans="1:54" ht="18.75" customHeight="1">
+      <c r="L15" s="12"/>
+      <c r="M15" s="15"/>
+      <c r="X15" s="12"/>
+      <c r="AB15" s="12"/>
+      <c r="AE15" s="12"/>
       <c r="AF15" s="12"/>
-      <c r="AG15" s="12"/>
       <c r="AP15" s="12"/>
     </row>
-    <row r="16" spans="1:53" ht="18.75" customHeight="1">
-      <c r="M16" s="12"/>
-      <c r="N16" s="15"/>
-      <c r="Y16" s="12"/>
-      <c r="AC16" s="12"/>
+    <row r="16" spans="1:54" ht="18.75" customHeight="1">
+      <c r="L16" s="12"/>
+      <c r="M16" s="15"/>
+      <c r="X16" s="12"/>
+      <c r="AB16" s="12"/>
+      <c r="AE16" s="12"/>
       <c r="AF16" s="12"/>
-      <c r="AG16" s="12"/>
       <c r="AP16" s="12"/>
     </row>
-    <row r="17" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M17" s="12"/>
-      <c r="N17" s="15"/>
-      <c r="Y17" s="12"/>
-      <c r="AC17" s="12"/>
+    <row r="17" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L17" s="12"/>
+      <c r="M17" s="15"/>
+      <c r="X17" s="12"/>
+      <c r="AB17" s="12"/>
+      <c r="AE17" s="12"/>
       <c r="AF17" s="12"/>
-      <c r="AG17" s="12"/>
       <c r="AP17" s="12"/>
     </row>
-    <row r="18" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M18" s="12"/>
-      <c r="N18" s="15"/>
-      <c r="Y18" s="12"/>
-      <c r="AC18" s="12"/>
+    <row r="18" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L18" s="12"/>
+      <c r="M18" s="15"/>
+      <c r="X18" s="12"/>
+      <c r="AB18" s="12"/>
+      <c r="AE18" s="12"/>
       <c r="AF18" s="12"/>
-      <c r="AG18" s="12"/>
       <c r="AP18" s="12"/>
     </row>
-    <row r="19" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M19" s="12"/>
-      <c r="N19" s="15"/>
-      <c r="Y19" s="12"/>
-      <c r="AC19" s="12"/>
+    <row r="19" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L19" s="12"/>
+      <c r="M19" s="15"/>
+      <c r="X19" s="12"/>
+      <c r="AB19" s="12"/>
+      <c r="AE19" s="12"/>
       <c r="AF19" s="12"/>
-      <c r="AG19" s="12"/>
       <c r="AP19" s="12"/>
     </row>
-    <row r="20" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M20" s="12"/>
-      <c r="N20" s="15"/>
-      <c r="Y20" s="12"/>
-      <c r="AC20" s="12"/>
+    <row r="20" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L20" s="12"/>
+      <c r="M20" s="15"/>
+      <c r="X20" s="12"/>
+      <c r="AB20" s="12"/>
+      <c r="AE20" s="12"/>
       <c r="AF20" s="12"/>
-      <c r="AG20" s="12"/>
       <c r="AP20" s="12"/>
     </row>
-    <row r="21" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M21" s="12"/>
-      <c r="N21" s="15"/>
-      <c r="Y21" s="12"/>
-      <c r="AC21" s="12"/>
+    <row r="21" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L21" s="12"/>
+      <c r="M21" s="15"/>
+      <c r="X21" s="12"/>
+      <c r="AB21" s="12"/>
+      <c r="AE21" s="12"/>
       <c r="AF21" s="12"/>
-      <c r="AG21" s="12"/>
       <c r="AP21" s="12"/>
     </row>
-    <row r="22" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M22" s="12"/>
-      <c r="N22" s="15"/>
-      <c r="Y22" s="12"/>
-      <c r="AC22" s="12"/>
+    <row r="22" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L22" s="12"/>
+      <c r="M22" s="15"/>
+      <c r="X22" s="12"/>
+      <c r="AB22" s="12"/>
+      <c r="AE22" s="12"/>
       <c r="AF22" s="12"/>
-      <c r="AG22" s="12"/>
       <c r="AP22" s="12"/>
     </row>
-    <row r="23" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M23" s="12"/>
-      <c r="N23" s="15"/>
-      <c r="Y23" s="12"/>
-      <c r="AC23" s="12"/>
+    <row r="23" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L23" s="12"/>
+      <c r="M23" s="15"/>
+      <c r="X23" s="12"/>
+      <c r="AB23" s="12"/>
+      <c r="AE23" s="12"/>
       <c r="AF23" s="12"/>
-      <c r="AG23" s="12"/>
       <c r="AP23" s="12"/>
     </row>
-    <row r="24" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M24" s="12"/>
-      <c r="N24" s="15"/>
-      <c r="Y24" s="12"/>
-      <c r="AC24" s="12"/>
+    <row r="24" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L24" s="12"/>
+      <c r="M24" s="15"/>
+      <c r="X24" s="12"/>
+      <c r="AB24" s="12"/>
+      <c r="AE24" s="12"/>
       <c r="AF24" s="12"/>
-      <c r="AG24" s="12"/>
       <c r="AP24" s="12"/>
     </row>
-    <row r="25" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M25" s="12"/>
-      <c r="N25" s="15"/>
-      <c r="Y25" s="12"/>
-      <c r="AC25" s="12"/>
+    <row r="25" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L25" s="12"/>
+      <c r="M25" s="15"/>
+      <c r="X25" s="12"/>
+      <c r="AB25" s="12"/>
+      <c r="AE25" s="12"/>
       <c r="AF25" s="12"/>
-      <c r="AG25" s="12"/>
       <c r="AP25" s="12"/>
     </row>
-    <row r="26" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M26" s="12"/>
-      <c r="N26" s="15"/>
-      <c r="Y26" s="12"/>
-      <c r="AC26" s="12"/>
+    <row r="26" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L26" s="12"/>
+      <c r="M26" s="15"/>
+      <c r="X26" s="12"/>
+      <c r="AB26" s="12"/>
+      <c r="AE26" s="12"/>
       <c r="AF26" s="12"/>
-      <c r="AG26" s="12"/>
       <c r="AP26" s="12"/>
     </row>
-    <row r="27" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M27" s="12"/>
-      <c r="N27" s="15"/>
-      <c r="Y27" s="12"/>
-      <c r="AC27" s="12"/>
+    <row r="27" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L27" s="12"/>
+      <c r="M27" s="15"/>
+      <c r="X27" s="12"/>
+      <c r="AB27" s="12"/>
+      <c r="AE27" s="12"/>
       <c r="AF27" s="12"/>
-      <c r="AG27" s="12"/>
       <c r="AP27" s="12"/>
     </row>
-    <row r="28" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M28" s="12"/>
-      <c r="N28" s="15"/>
-      <c r="Y28" s="12"/>
-      <c r="AC28" s="12"/>
+    <row r="28" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L28" s="12"/>
+      <c r="M28" s="15"/>
+      <c r="X28" s="12"/>
+      <c r="AB28" s="12"/>
+      <c r="AE28" s="12"/>
       <c r="AF28" s="12"/>
-      <c r="AG28" s="12"/>
       <c r="AP28" s="12"/>
     </row>
-    <row r="29" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M29" s="12"/>
-      <c r="N29" s="15"/>
-      <c r="Y29" s="12"/>
-      <c r="AC29" s="12"/>
+    <row r="29" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L29" s="12"/>
+      <c r="M29" s="15"/>
+      <c r="X29" s="12"/>
+      <c r="AB29" s="12"/>
+      <c r="AE29" s="12"/>
       <c r="AF29" s="12"/>
-      <c r="AG29" s="12"/>
       <c r="AP29" s="12"/>
     </row>
-    <row r="30" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M30" s="12"/>
-      <c r="N30" s="15"/>
-      <c r="Y30" s="12"/>
-      <c r="AC30" s="12"/>
+    <row r="30" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L30" s="12"/>
+      <c r="M30" s="15"/>
+      <c r="X30" s="12"/>
+      <c r="AB30" s="12"/>
+      <c r="AE30" s="12"/>
       <c r="AF30" s="12"/>
-      <c r="AG30" s="12"/>
       <c r="AP30" s="12"/>
     </row>
-    <row r="31" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M31" s="12"/>
-      <c r="N31" s="15"/>
-      <c r="Y31" s="12"/>
-      <c r="AC31" s="12"/>
+    <row r="31" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L31" s="12"/>
+      <c r="M31" s="15"/>
+      <c r="X31" s="12"/>
+      <c r="AB31" s="12"/>
+      <c r="AE31" s="12"/>
       <c r="AF31" s="12"/>
-      <c r="AG31" s="12"/>
       <c r="AP31" s="12"/>
     </row>
-    <row r="32" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M32" s="12"/>
-      <c r="N32" s="15"/>
-      <c r="Y32" s="12"/>
-      <c r="AC32" s="12"/>
+    <row r="32" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L32" s="12"/>
+      <c r="M32" s="15"/>
+      <c r="X32" s="12"/>
+      <c r="AB32" s="12"/>
+      <c r="AE32" s="12"/>
       <c r="AF32" s="12"/>
-      <c r="AG32" s="12"/>
       <c r="AP32" s="12"/>
     </row>
-    <row r="33" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M33" s="12"/>
-      <c r="N33" s="15"/>
-      <c r="Y33" s="12"/>
-      <c r="AC33" s="12"/>
+    <row r="33" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L33" s="12"/>
+      <c r="M33" s="15"/>
+      <c r="X33" s="12"/>
+      <c r="AB33" s="12"/>
+      <c r="AE33" s="12"/>
       <c r="AF33" s="12"/>
-      <c r="AG33" s="12"/>
       <c r="AP33" s="12"/>
     </row>
-    <row r="34" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M34" s="12"/>
-      <c r="N34" s="15"/>
-      <c r="Y34" s="12"/>
-      <c r="AC34" s="12"/>
+    <row r="34" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L34" s="12"/>
+      <c r="M34" s="15"/>
+      <c r="X34" s="12"/>
+      <c r="AB34" s="12"/>
+      <c r="AE34" s="12"/>
       <c r="AF34" s="12"/>
-      <c r="AG34" s="12"/>
       <c r="AP34" s="12"/>
     </row>
-    <row r="35" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M35" s="12"/>
-      <c r="N35" s="15"/>
-      <c r="Y35" s="12"/>
-      <c r="AC35" s="12"/>
+    <row r="35" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L35" s="12"/>
+      <c r="M35" s="15"/>
+      <c r="X35" s="12"/>
+      <c r="AB35" s="12"/>
+      <c r="AE35" s="12"/>
       <c r="AF35" s="12"/>
-      <c r="AG35" s="12"/>
       <c r="AP35" s="12"/>
     </row>
-    <row r="36" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M36" s="12"/>
-      <c r="N36" s="15"/>
-      <c r="Y36" s="12"/>
-      <c r="AC36" s="12"/>
+    <row r="36" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L36" s="12"/>
+      <c r="M36" s="15"/>
+      <c r="X36" s="12"/>
+      <c r="AB36" s="12"/>
+      <c r="AE36" s="12"/>
       <c r="AF36" s="12"/>
-      <c r="AG36" s="12"/>
       <c r="AP36" s="12"/>
     </row>
-    <row r="37" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M37" s="12"/>
-      <c r="N37" s="15"/>
-      <c r="Y37" s="12"/>
-      <c r="AC37" s="12"/>
+    <row r="37" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L37" s="12"/>
+      <c r="M37" s="15"/>
+      <c r="X37" s="12"/>
+      <c r="AB37" s="12"/>
+      <c r="AE37" s="12"/>
       <c r="AF37" s="12"/>
-      <c r="AG37" s="12"/>
       <c r="AP37" s="12"/>
     </row>
-    <row r="38" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M38" s="12"/>
-      <c r="N38" s="15"/>
-      <c r="Y38" s="12"/>
-      <c r="AC38" s="12"/>
+    <row r="38" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L38" s="12"/>
+      <c r="M38" s="15"/>
+      <c r="X38" s="12"/>
+      <c r="AB38" s="12"/>
+      <c r="AE38" s="12"/>
       <c r="AF38" s="12"/>
-      <c r="AG38" s="12"/>
       <c r="AP38" s="12"/>
     </row>
-    <row r="39" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M39" s="12"/>
-      <c r="N39" s="15"/>
-      <c r="Y39" s="12"/>
-      <c r="AC39" s="12"/>
+    <row r="39" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L39" s="12"/>
+      <c r="M39" s="15"/>
+      <c r="X39" s="12"/>
+      <c r="AB39" s="12"/>
+      <c r="AE39" s="12"/>
       <c r="AF39" s="12"/>
-      <c r="AG39" s="12"/>
       <c r="AP39" s="12"/>
     </row>
-    <row r="40" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M40" s="12"/>
-      <c r="N40" s="15"/>
-      <c r="Y40" s="12"/>
-      <c r="AC40" s="12"/>
+    <row r="40" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L40" s="12"/>
+      <c r="M40" s="15"/>
+      <c r="X40" s="12"/>
+      <c r="AB40" s="12"/>
+      <c r="AE40" s="12"/>
       <c r="AF40" s="12"/>
-      <c r="AG40" s="12"/>
       <c r="AP40" s="12"/>
     </row>
-    <row r="41" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M41" s="12"/>
-      <c r="N41" s="15"/>
-      <c r="Y41" s="12"/>
-      <c r="AC41" s="12"/>
+    <row r="41" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L41" s="12"/>
+      <c r="M41" s="15"/>
+      <c r="X41" s="12"/>
+      <c r="AB41" s="12"/>
+      <c r="AE41" s="12"/>
       <c r="AF41" s="12"/>
-      <c r="AG41" s="12"/>
       <c r="AP41" s="12"/>
     </row>
-    <row r="42" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M42" s="12"/>
-      <c r="N42" s="15"/>
-      <c r="Y42" s="12"/>
-      <c r="AC42" s="12"/>
+    <row r="42" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L42" s="12"/>
+      <c r="M42" s="15"/>
+      <c r="X42" s="12"/>
+      <c r="AB42" s="12"/>
+      <c r="AE42" s="12"/>
       <c r="AF42" s="12"/>
-      <c r="AG42" s="12"/>
       <c r="AP42" s="12"/>
     </row>
-    <row r="43" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M43" s="12"/>
-      <c r="N43" s="15"/>
-      <c r="Y43" s="12"/>
-      <c r="AC43" s="12"/>
+    <row r="43" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L43" s="12"/>
+      <c r="M43" s="15"/>
+      <c r="X43" s="12"/>
+      <c r="AB43" s="12"/>
+      <c r="AE43" s="12"/>
       <c r="AF43" s="12"/>
-      <c r="AG43" s="12"/>
       <c r="AP43" s="12"/>
     </row>
-    <row r="44" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M44" s="12"/>
-      <c r="N44" s="15"/>
-      <c r="Y44" s="12"/>
-      <c r="AC44" s="12"/>
+    <row r="44" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L44" s="12"/>
+      <c r="M44" s="15"/>
+      <c r="X44" s="12"/>
+      <c r="AB44" s="12"/>
+      <c r="AE44" s="12"/>
       <c r="AF44" s="12"/>
-      <c r="AG44" s="12"/>
       <c r="AP44" s="12"/>
     </row>
-    <row r="45" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M45" s="12"/>
-      <c r="N45" s="15"/>
-      <c r="Y45" s="12"/>
-      <c r="AC45" s="12"/>
+    <row r="45" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L45" s="12"/>
+      <c r="M45" s="15"/>
+      <c r="X45" s="12"/>
+      <c r="AB45" s="12"/>
+      <c r="AE45" s="12"/>
       <c r="AF45" s="12"/>
-      <c r="AG45" s="12"/>
       <c r="AP45" s="12"/>
     </row>
-    <row r="46" spans="13:42" ht="18.75" customHeight="1">
-      <c r="M46" s="12"/>
-      <c r="N46" s="15"/>
-      <c r="Y46" s="12"/>
-      <c r="AC46" s="12"/>
+    <row r="46" spans="12:42" ht="18.75" customHeight="1">
+      <c r="L46" s="12"/>
+      <c r="M46" s="15"/>
+      <c r="X46" s="12"/>
+      <c r="AB46" s="12"/>
+      <c r="AE46" s="12"/>
       <c r="AF46" s="12"/>
-      <c r="AG46" s="12"/>
       <c r="AP46" s="12"/>
     </row>
   </sheetData>
@@ -3917,61 +3926,6 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
     <mergeCell ref="B75:C75"/>
     <mergeCell ref="B76:C76"/>
     <mergeCell ref="B77:C77"/>
@@ -3980,6 +3934,61 @@
     <mergeCell ref="B72:C72"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>